<commit_message>
Added FORD PBT code
</commit_message>
<xml_diff>
--- a/OOH_PBT/OOH_PBT_Issue_Upload_To_Sharepoint/Data/Config.xlsx
+++ b/OOH_PBT/OOH_PBT_Issue_Upload_To_Sharepoint/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1Files\UPProjects\OOH_PBT\OOH_PBT_Issue_Upload_To_Sharepoint\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD3A605-25E6-4D2D-A3AC-D44E4614DC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180A95DC-DE40-41FC-B7F5-3047234B92A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="20775" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -156,10 +156,10 @@
     <t>https://insidemedia.sharepoint.com/sites/GMUSA-KineticFinanceAutomation/</t>
   </si>
   <si>
-    <t>Data Source=eussqsvgrmusafinance01.database.windows.net;Initial Catalog=eussqdbgrmusaapoohdev01;User ID=NA_sqlusr_AP_OOH_DEV_01;Password=JFcRxniU2hETyEgCQxM3</t>
-  </si>
-  <si>
     <t>C:\Users\NTMGRM.RPA1\Desktop\OOH_PBT_Exception_Screenshots\</t>
+  </si>
+  <si>
+    <t>Data Source=eussqsvgrmusafinance01.database.windows.net;Initial Catalog=eussqdbgrmusaapooh01;User ID=NA_AP_OOH_DBAUSR_01;Password=n28UxD8NVZAqdFMjBHnd</t>
   </si>
 </sst>
 </file>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -626,7 +626,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>37</v>
@@ -648,7 +648,7 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>